<commit_message>
Roles and permission changes, make nurse naming less restrictive #108
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/contact/nurse-create.xlsx
+++ b/config/itech-aurum/forms/contact/nurse-create.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\contact\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-108\itech-aurum\forms\contact\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2666EBC9-002F-4513-857F-91FB8F61A819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6F91DA9-4D56-4B97-94FD-9F74D84170E0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="67">
   <si>
     <t>type</t>
   </si>
@@ -96,12 +96,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>regex(., "^[a-zA-Z\'\s]+$")</t>
-  </si>
-  <si>
-    <t>Please type in name characters e.g letters and space.</t>
   </si>
   <si>
     <t>calculate</t>
@@ -557,7 +551,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -630,7 +624,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1" t="s">
@@ -733,10 +727,10 @@
         <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -779,12 +773,8 @@
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
-      <c r="I6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -802,13 +792,13 @@
     </row>
     <row r="7" spans="1:24" ht="12.75" customHeight="1">
       <c r="A7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="3" t="s">
@@ -840,7 +830,7 @@
     </row>
     <row r="8" spans="1:24" ht="12.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1863,7 +1853,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1879,134 +1869,134 @@
     </row>
     <row r="3" spans="1:3" ht="15.75">
       <c r="A3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75">
       <c r="A4" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75">
       <c r="A7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75">
       <c r="A9" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
       <c r="A11" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
       <c r="A12" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
       <c r="A15" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1"/>
@@ -3005,19 +2995,19 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1">
       <c r="A1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>60</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
@@ -3032,19 +3022,19 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1">
       <c r="A2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="E2" s="11" t="s">
         <v>63</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>

</xml_diff>